<commit_message>
Add tool to verify retirement periods (S 3^3)
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B9576F-3076-4646-AED2-531379ECE18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7ADAA97-310E-43F6-B440-F7C538606254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technologies" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="406">
   <si>
     <t>tech</t>
   </si>
@@ -1277,6 +1277,9 @@
   <si>
     <t>USED ATB 22- Could use (State Energy Data System (SEDS): 2022 + Wood and biomass waste + Price and Expenditures + WWEID https://www.eia.gov/state/seds/seds-data-fuel-prev.php 2.5M$/PJ)</t>
   </si>
+  <si>
+    <t>Temporary modification original value was 33</t>
+  </si>
 </sst>
 </file>
 
@@ -2374,6 +2377,9 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2381,9 +2387,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4369,18 +4372,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="47.25" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
@@ -6046,9 +6049,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C008AD2-9FC6-4B50-8E5B-D9A0AF2799B1}">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6081,7 +6084,7 @@
         <v>290</v>
       </c>
       <c r="B2">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -6115,7 +6118,7 @@
         <v>289</v>
       </c>
       <c r="B4">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -6132,7 +6135,7 @@
         <v>292</v>
       </c>
       <c r="B5">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -6166,7 +6169,7 @@
         <v>294</v>
       </c>
       <c r="B7">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>20</v>
@@ -6183,7 +6186,7 @@
         <v>295</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>20</v>
@@ -6200,7 +6203,7 @@
         <v>296</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C9">
         <v>20</v>
@@ -6285,7 +6288,7 @@
         <v>299</v>
       </c>
       <c r="B14">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>20</v>
@@ -6319,7 +6322,7 @@
         <v>301</v>
       </c>
       <c r="B16">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -6387,7 +6390,7 @@
         <v>305</v>
       </c>
       <c r="B20">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C20">
         <v>20</v>
@@ -6413,7 +6416,7 @@
         <v>359</v>
       </c>
       <c r="E21" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -7005,8 +7008,8 @@
   <dimension ref="A1:L124"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -11796,13 +11799,13 @@
       <c r="N1" t="s">
         <v>400</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="Q1" s="21" t="s">
         <v>401</v>
       </c>
-      <c r="R1" s="24" t="s">
+      <c r="R1" s="21" t="s">
         <v>402</v>
       </c>
     </row>
@@ -11852,14 +11855,14 @@
         <f>J2*C2</f>
         <v>11022</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="P2" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="Q2" s="24">
+      <c r="Q2" s="21">
         <f>SUMIF($M$2:$M$125, P2, $C$2:$C$125)</f>
         <v>9294</v>
       </c>
-      <c r="R2" s="24">
+      <c r="R2" s="21">
         <f>SUMIF($M$2:$M$125, P2, $N$2:$N$125)/Q2</f>
         <v>55.796858188078332</v>
       </c>
@@ -11910,14 +11913,14 @@
         <f t="shared" ref="N3:N66" si="2">J3*C3</f>
         <v>16058</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="Q3" s="24">
+      <c r="Q3" s="21">
         <f t="shared" ref="Q3:Q8" si="3">SUMIF($M$2:$M$125, P3, $C$2:$C$125)</f>
         <v>5184</v>
       </c>
-      <c r="R3" s="24">
+      <c r="R3" s="21">
         <f t="shared" ref="R3:R8" si="4">SUMIF($M$2:$M$125, P3, $N$2:$N$125)/Q3</f>
         <v>41.582754629629626</v>
       </c>
@@ -11968,14 +11971,14 @@
         <f t="shared" si="2"/>
         <v>7400</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="Q4" s="24">
+      <c r="Q4" s="21">
         <f t="shared" si="3"/>
         <v>1876</v>
       </c>
-      <c r="R4" s="24">
+      <c r="R4" s="21">
         <f t="shared" si="4"/>
         <v>37.380597014925371</v>
       </c>
@@ -12026,14 +12029,14 @@
         <f t="shared" si="2"/>
         <v>7400</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="P5" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="Q5" s="24">
+      <c r="Q5" s="21">
         <f t="shared" si="3"/>
         <v>838.3</v>
       </c>
-      <c r="R5" s="24">
+      <c r="R5" s="21">
         <f t="shared" si="4"/>
         <v>108.87677442443039</v>
       </c>
@@ -12084,14 +12087,14 @@
         <f t="shared" si="2"/>
         <v>7600</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="Q6" s="24">
+      <c r="Q6" s="21">
         <f t="shared" si="3"/>
         <v>232</v>
       </c>
-      <c r="R6" s="24">
+      <c r="R6" s="21">
         <f t="shared" si="4"/>
         <v>68.706896551724142</v>
       </c>
@@ -12142,14 +12145,14 @@
         <f t="shared" si="2"/>
         <v>3600</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="Q7" s="24">
+      <c r="Q7" s="21">
         <f t="shared" si="3"/>
         <v>2937</v>
       </c>
-      <c r="R7" s="24">
+      <c r="R7" s="21">
         <f t="shared" si="4"/>
         <v>59.343547837929862</v>
       </c>
@@ -12200,14 +12203,14 @@
         <f t="shared" si="2"/>
         <v>7410</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="Q8" s="24">
+      <c r="Q8" s="21">
         <f t="shared" si="3"/>
         <v>2763</v>
       </c>
-      <c r="R8" s="24">
+      <c r="R8" s="21">
         <f t="shared" si="4"/>
         <v>37.155266015200866</v>
       </c>
@@ -35684,7 +35687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F64963-0CDD-4BE6-B0AC-E6FD0D7CCBEC}">
   <dimension ref="A1:AI94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>

</xml_diff>

<commit_message>
Cost Increase and mph as well (rmv)
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
@@ -17780,9 +17780,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57:E57"/>
+      <selection pane="bottomLeft" activeCell="E74" sqref="E74:AI74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
@@ -25620,128 +25620,128 @@
         <v>409</v>
       </c>
       <c r="E74" s="12">
-        <f>8012*0.2</f>
-        <v>1602.4</v>
+        <f>8012*0.15</f>
+        <v>1201.8</v>
       </c>
       <c r="F74" s="12">
-        <f t="shared" ref="F74:AI74" si="0">8012*0.2</f>
-        <v>1602.4</v>
+        <f t="shared" ref="F74:AI74" si="0">8012*0.15</f>
+        <v>1201.8</v>
       </c>
       <c r="G74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="H74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="I74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="J74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="K74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="L74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="M74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="N74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="O74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="P74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="Q74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="R74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="S74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="T74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="U74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="V74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="W74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="X74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="Y74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="Z74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="AA74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="AB74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="AC74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="AD74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="AE74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="AF74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="AG74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="AH74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
       <c r="AI74" s="12">
         <f t="shared" si="0"/>
-        <v>1602.4</v>
+        <v>1201.8</v>
       </c>
     </row>
   </sheetData>
@@ -35845,128 +35845,128 @@
         <v>410</v>
       </c>
       <c r="E95" s="14">
-        <f>183*0.2</f>
-        <v>36.6</v>
+        <f>183*0.15</f>
+        <v>27.45</v>
       </c>
       <c r="F95" s="14">
-        <f t="shared" ref="F95:AI95" si="0">183*0.2</f>
-        <v>36.6</v>
+        <f t="shared" ref="F95:AI95" si="0">183*0.15</f>
+        <v>27.45</v>
       </c>
       <c r="G95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="H95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="I95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="J95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="K95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="L95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="M95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="N95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="O95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="P95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="Q95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="R95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="S95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="T95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="U95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="V95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="W95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="X95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="Y95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="Z95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="AA95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="AB95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="AC95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="AD95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="AE95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="AF95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="AG95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="AH95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
       <c r="AI95" s="14">
         <f t="shared" si="0"/>
-        <v>36.6</v>
+        <v>27.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filter for Existing tech not used (due lifetime)
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7ADAA97-310E-43F6-B440-F7C538606254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F71260-9EA8-4419-8BED-BB7D780B1CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6051,7 +6051,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6390,7 +6390,7 @@
         <v>305</v>
       </c>
       <c r="B20">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C20">
         <v>20</v>
@@ -6407,7 +6407,7 @@
         <v>306</v>
       </c>
       <c r="B21">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C21">
         <v>20</v>

</xml_diff>

<commit_message>
Update Emissions - (SR)
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\8-11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8018DB-D98B-495D-9CA2-559FB015E993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E178DF-2BD9-4D0B-96E5-C6CB12510117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="935" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technologies" sheetId="1" r:id="rId1"/>
@@ -3125,12 +3125,12 @@
       <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" customWidth="1"/>
-    <col min="2" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="76.85546875" customWidth="1"/>
-    <col min="5" max="5" width="112.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.3984375" customWidth="1"/>
+    <col min="2" max="3" width="13.59765625" customWidth="1"/>
+    <col min="4" max="4" width="76.86328125" customWidth="1"/>
+    <col min="5" max="5" width="112.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="24" customFormat="1" ht="29.25" customHeight="1">
@@ -3974,7 +3974,7 @@
       <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -4000,9 +4000,9 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="26.59765625" customWidth="1"/>
     <col min="2" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4438,14 +4438,14 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="84.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.86328125" customWidth="1"/>
+    <col min="2" max="2" width="21.59765625" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" customWidth="1"/>
+    <col min="4" max="4" width="84.265625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="8" width="29.140625" customWidth="1"/>
+    <col min="6" max="8" width="29.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="47.25" customHeight="1">
@@ -5435,7 +5435,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="30">
+    <row r="52" spans="1:3" ht="28.5">
       <c r="A52" s="4" t="s">
         <v>31</v>
       </c>
@@ -5459,17 +5459,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F425B7AA-21D1-411D-A9AF-54EA873F398D}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.1328125" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.86328125" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5613,12 +5613,12 @@
       <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="112.85546875" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.3984375" customWidth="1"/>
+    <col min="2" max="4" width="14.59765625" customWidth="1"/>
+    <col min="5" max="5" width="112.86328125" customWidth="1"/>
+    <col min="6" max="8" width="9.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6132,12 +6132,12 @@
       <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="61.140625" customWidth="1"/>
-    <col min="5" max="5" width="112.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.1328125" customWidth="1"/>
+    <col min="2" max="3" width="13.59765625" customWidth="1"/>
+    <col min="4" max="4" width="61.1328125" customWidth="1"/>
+    <col min="5" max="5" width="112.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7090,11 +7090,11 @@
       <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18.1328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="8" width="18.140625" style="2"/>
-    <col min="9" max="9" width="40.28515625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="18.140625" style="2"/>
+    <col min="1" max="8" width="18.1328125" style="2"/>
+    <col min="9" max="9" width="40.265625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="18.1328125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
@@ -11827,11 +11827,11 @@
       <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18.1328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="8" max="9" width="23.85546875" customWidth="1"/>
-    <col min="11" max="12" width="18.140625" style="2"/>
-    <col min="18" max="18" width="36.42578125" customWidth="1"/>
+    <col min="8" max="9" width="23.86328125" customWidth="1"/>
+    <col min="11" max="12" width="18.1328125" style="2"/>
+    <col min="18" max="18" width="36.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1">
@@ -17810,14 +17810,14 @@
       <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" style="12" customWidth="1"/>
-    <col min="5" max="35" width="6.42578125" style="14" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="12.59765625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.3984375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.86328125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="33.73046875" style="12" customWidth="1"/>
+    <col min="5" max="35" width="6.3984375" style="14" customWidth="1"/>
+    <col min="36" max="16384" width="9.1328125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -25683,14 +25683,14 @@
       <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" style="12" customWidth="1"/>
-    <col min="5" max="35" width="6.42578125" style="14" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="15.3984375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16.265625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="29.1328125" style="12" customWidth="1"/>
+    <col min="5" max="35" width="6.3984375" style="14" customWidth="1"/>
+    <col min="36" max="16384" width="9.1328125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -35762,20 +35762,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F64963-0CDD-4BE6-B0AC-E6FD0D7CCBEC}">
   <dimension ref="A1:AJ94"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23:AJ23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="12" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="22.86328125" style="12" customWidth="1"/>
     <col min="3" max="3" width="15" style="12" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="12" customWidth="1"/>
-    <col min="6" max="36" width="6.42578125" style="14" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="12"/>
+    <col min="4" max="4" width="40.73046875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.73046875" style="12" customWidth="1"/>
+    <col min="6" max="36" width="6.3984375" style="14" customWidth="1"/>
+    <col min="37" max="16384" width="9.1328125" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="26" customFormat="1" ht="23.25" customHeight="1">
@@ -37648,7 +37648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="12">
+    <row r="18" spans="1:36" ht="11.65">
       <c r="A18" s="12" t="s">
         <v>41</v>
       </c>
@@ -38215,128 +38215,128 @@
         <v>1</v>
       </c>
       <c r="F23" s="22">
-        <f>11*1.17*(10^-3)/1.10231</f>
-        <v>1.1675481488873367E-2</v>
+        <f>11*1.17*(10^-3)</f>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="G23" s="22">
-        <f t="shared" ref="G23:AJ23" si="0">11*1.17*(10^-3)/1.10231</f>
-        <v>1.1675481488873367E-2</v>
+        <f t="shared" ref="G23:AJ23" si="0">11*1.17*(10^-3)</f>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="H23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="I23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="J23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="K23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="L23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="M23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="N23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="O23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="P23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="Q23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="R23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="S23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="T23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="U23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="V23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="W23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="X23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="Y23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="Z23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AA23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AB23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AC23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AD23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AE23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AF23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AG23" s="22">
-        <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <f>11*1.17*(10^-3)</f>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AH23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AI23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
       <c r="AJ23" s="22">
         <f t="shared" si="0"/>
-        <v>1.1675481488873367E-2</v>
+        <v>1.2869999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:36" ht="12.95" customHeight="1">
@@ -46164,10 +46164,10 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="114.7109375" customWidth="1"/>
+    <col min="1" max="3" width="18.59765625" customWidth="1"/>
+    <col min="4" max="4" width="114.73046875" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
New Wind CF format and max/min format
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor\Desktop\8-11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E178DF-2BD9-4D0B-96E5-C6CB12510117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CC7222-67FA-4520-AC45-3B90BE88149D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="935" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technologies" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2945" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="434">
   <si>
     <t>tech</t>
   </si>
@@ -1341,6 +1341,30 @@
   <si>
     <t>For Energy Losses:  https://www.eia.gov/tools/faqs/faq.php?id=105&amp;t=3</t>
   </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CF by season- NC Statistics </t>
+  </si>
+  <si>
+    <t>https://www.eia.gov/electricity/state/archive/2020/northcarolina/</t>
+  </si>
 </sst>
 </file>
 
@@ -2458,10 +2482,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3121,16 +3145,16 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="33.3984375" customWidth="1"/>
-    <col min="2" max="3" width="13.59765625" customWidth="1"/>
-    <col min="4" max="4" width="76.86328125" customWidth="1"/>
-    <col min="5" max="5" width="112.86328125" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="76.85546875" customWidth="1"/>
+    <col min="5" max="5" width="112.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="24" customFormat="1" ht="29.25" customHeight="1">
@@ -3974,7 +3998,7 @@
       <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -3994,24 +4018,24 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904DECE4-C220-4D32-A501-0A9FE9B4057C}">
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.59765625" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:16">
       <c r="A2" s="6" t="s">
         <v>96</v>
       </c>
@@ -4028,7 +4052,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -4045,7 +4069,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -4062,7 +4086,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -4079,7 +4103,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -4087,7 +4111,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -4095,7 +4119,7 @@
         <v>108.8</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -4103,7 +4127,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>75</v>
       </c>
@@ -4111,31 +4135,72 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>56</v>
       </c>
       <c r="B10" s="2">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="K10" s="28" t="s">
+        <v>432</v>
+      </c>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>79</v>
       </c>
       <c r="B11" s="2">
         <v>70.599999999999994</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="L11" t="s">
+        <v>426</v>
+      </c>
+      <c r="M11" t="s">
+        <v>427</v>
+      </c>
+      <c r="N11" t="s">
+        <v>428</v>
+      </c>
+      <c r="O11" t="s">
+        <v>429</v>
+      </c>
+      <c r="P11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="2">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="K12" t="s">
+        <v>430</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="N12" s="2">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="O12" s="2">
+        <v>0.34100000000000003</v>
+      </c>
+      <c r="P12" s="15">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -4148,8 +4213,26 @@
       <c r="D13" s="2">
         <v>212</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="K13" t="s">
+        <v>430</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.498</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="P13" s="15">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -4158,8 +4241,26 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="K14" t="s">
+        <v>430</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.378</v>
+      </c>
+      <c r="N14" s="2">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="O14" s="2">
+        <v>20.9</v>
+      </c>
+      <c r="P14" s="15">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>91</v>
       </c>
@@ -4168,8 +4269,26 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="K15" t="s">
+        <v>430</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.313</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="P15" s="15">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -4178,8 +4297,26 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="K16" t="s">
+        <v>430</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.251</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.189</v>
+      </c>
+      <c r="P16" s="15">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" t="s">
         <v>90</v>
       </c>
@@ -4188,8 +4325,11 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="K17" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -4199,7 +4339,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:11">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -4209,7 +4349,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -4219,7 +4359,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:11">
       <c r="A21" t="s">
         <v>89</v>
       </c>
@@ -4229,7 +4369,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:11">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -4246,7 +4386,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -4254,7 +4394,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -4262,7 +4402,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -4270,7 +4410,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:11">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -4278,7 +4418,7 @@
         <v>9.6</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:11">
       <c r="A27" t="s">
         <v>66</v>
       </c>
@@ -4286,7 +4426,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:11">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -4294,7 +4434,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:11">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -4302,7 +4442,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:11">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -4310,7 +4450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:11">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -4318,7 +4458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:11">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -4426,6 +4566,9 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B108">
     <sortCondition descending="1" ref="B108"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="K10:P10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4438,23 +4581,23 @@
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" customWidth="1"/>
-    <col min="2" max="2" width="21.59765625" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" customWidth="1"/>
-    <col min="4" max="4" width="84.265625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="84.28515625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="8" width="29.1328125" customWidth="1"/>
+    <col min="6" max="8" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="47.25" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="1"/>
       <c r="F1" s="30" t="s">
         <v>26</v>
@@ -5435,7 +5578,7 @@
         <v>2037</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="28.5">
+    <row r="52" spans="1:3" ht="30">
       <c r="A52" s="4" t="s">
         <v>31</v>
       </c>
@@ -5463,13 +5606,13 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="16.265625" customWidth="1"/>
-    <col min="3" max="3" width="19.1328125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="16.86328125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5608,17 +5751,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A32AD897-F683-4767-9F8A-BBAC538730FF}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.3984375" customWidth="1"/>
-    <col min="2" max="4" width="14.59765625" customWidth="1"/>
-    <col min="5" max="5" width="112.86328125" customWidth="1"/>
-    <col min="6" max="8" width="9.1328125" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="112.85546875" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6132,12 +6275,12 @@
       <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.1328125" customWidth="1"/>
-    <col min="2" max="3" width="13.59765625" customWidth="1"/>
-    <col min="4" max="4" width="61.1328125" customWidth="1"/>
-    <col min="5" max="5" width="112.86328125" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="61.140625" customWidth="1"/>
+    <col min="5" max="5" width="112.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7090,11 +7233,11 @@
       <selection pane="bottomLeft" activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.1328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="8" width="18.1328125" style="2"/>
-    <col min="9" max="9" width="40.265625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="18.1328125" style="2"/>
+    <col min="1" max="8" width="18.140625" style="2"/>
+    <col min="9" max="9" width="40.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="18.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
@@ -11827,11 +11970,11 @@
       <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.1328125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="8" max="9" width="23.86328125" customWidth="1"/>
-    <col min="11" max="12" width="18.1328125" style="2"/>
-    <col min="18" max="18" width="36.3984375" customWidth="1"/>
+    <col min="8" max="9" width="23.85546875" customWidth="1"/>
+    <col min="11" max="12" width="18.140625" style="2"/>
+    <col min="18" max="18" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1">
@@ -17810,14 +17953,14 @@
       <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="30.3984375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="6.86328125" style="12" customWidth="1"/>
-    <col min="4" max="4" width="33.73046875" style="12" customWidth="1"/>
-    <col min="5" max="35" width="6.3984375" style="14" customWidth="1"/>
-    <col min="36" max="16384" width="9.1328125" style="12"/>
+    <col min="1" max="1" width="12.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" style="12" customWidth="1"/>
+    <col min="5" max="35" width="6.42578125" style="14" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -25683,14 +25826,14 @@
       <selection pane="bottomLeft" activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.65"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="15.3984375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="25.265625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="16.265625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="29.1328125" style="12" customWidth="1"/>
-    <col min="5" max="35" width="6.3984375" style="14" customWidth="1"/>
-    <col min="36" max="16384" width="9.1328125" style="12"/>
+    <col min="1" max="1" width="15.42578125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" style="12" customWidth="1"/>
+    <col min="5" max="35" width="6.42578125" style="14" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
@@ -35762,20 +35905,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F64963-0CDD-4BE6-B0AC-E6FD0D7CCBEC}">
   <dimension ref="A1:AJ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23:AJ23"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.95" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.95" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.59765625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="22.86328125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="12" customWidth="1"/>
     <col min="3" max="3" width="15" style="12" customWidth="1"/>
-    <col min="4" max="4" width="40.73046875" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.73046875" style="12" customWidth="1"/>
-    <col min="6" max="36" width="6.3984375" style="14" customWidth="1"/>
-    <col min="37" max="16384" width="9.1328125" style="12"/>
+    <col min="4" max="4" width="40.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" style="12" customWidth="1"/>
+    <col min="6" max="36" width="6.42578125" style="14" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="26" customFormat="1" ht="23.25" customHeight="1">
@@ -37648,7 +37791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="11.65">
+    <row r="18" spans="1:36" ht="12">
       <c r="A18" s="12" t="s">
         <v>41</v>
       </c>
@@ -46164,10 +46307,10 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="18.59765625" customWidth="1"/>
-    <col min="4" max="4" width="114.73046875" customWidth="1"/>
+    <col min="1" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="114.7109375" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Some Updates on the OBJ function
</commit_message>
<xml_diff>
--- a/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
+++ b/CreateDB_NC/InputData/ExcelUserData/UserDataPart1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remote\Desktop\Projects\TemoaHurricane_OEA\TEMOA_GIT\TemoaHurricane_V2\CreateDB_NC\InputData\ExcelUserData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A6D202-B68D-4E97-939C-B926D520E607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D754A5-371B-4CDE-8910-A96A33987D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="935" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="technologies" sheetId="1" r:id="rId1"/>
@@ -3726,7 +3726,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4798,7 +4798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F3BFE1-3002-4175-B18A-F0D552E5CBB3}">
   <dimension ref="A1:AG74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -11486,7 +11486,7 @@
   <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N63" sqref="N63"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14120,8 +14120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C343DE-8FD7-43B0-8B91-52EA75A17858}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14311,7 +14311,7 @@
         <v>2022</v>
       </c>
       <c r="D8" s="2">
-        <v>1</v>
+        <v>2.9</v>
       </c>
       <c r="E8" t="s">
         <v>459</v>
@@ -14334,7 +14334,7 @@
         <v>2022</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E9" t="s">
         <v>459</v>
@@ -14357,7 +14357,7 @@
         <v>2022</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>459</v>
@@ -14380,7 +14380,7 @@
         <v>2022</v>
       </c>
       <c r="D11" s="2">
-        <v>1</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E11" t="s">
         <v>459</v>
@@ -14403,7 +14403,7 @@
         <v>2022</v>
       </c>
       <c r="D12" s="2">
-        <v>1</v>
+        <v>3.2</v>
       </c>
       <c r="E12" t="s">
         <v>459</v>
@@ -14426,7 +14426,7 @@
         <v>2022</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>19.5</v>
       </c>
       <c r="E13" t="s">
         <v>459</v>
@@ -14449,7 +14449,7 @@
         <v>2022</v>
       </c>
       <c r="D14" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="E14" t="s">
         <v>459</v>
@@ -14472,7 +14472,7 @@
         <v>2022</v>
       </c>
       <c r="D15" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="E15" t="s">
         <v>459</v>
@@ -14495,7 +14495,7 @@
         <v>2022</v>
       </c>
       <c r="D16" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="E16" t="s">
         <v>459</v>
@@ -14518,7 +14518,7 @@
         <v>2022</v>
       </c>
       <c r="D17" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="E17" t="s">
         <v>459</v>
@@ -14541,7 +14541,7 @@
         <v>2022</v>
       </c>
       <c r="D18" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="E18" t="s">
         <v>459</v>
@@ -14564,7 +14564,7 @@
         <v>2022</v>
       </c>
       <c r="D19" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="E19" t="s">
         <v>459</v>
@@ -14748,7 +14748,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A43" sqref="A43:D43"/>
     </sheetView>
   </sheetViews>
@@ -15484,8 +15484,8 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="A12:A13 A3"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49:C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27387,7 +27387,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B89" sqref="B76:B89"/>
+      <selection pane="bottomLeft" activeCell="B67" sqref="B67:G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
@@ -37026,7 +37026,7 @@
   <dimension ref="A1:AI110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B97" sqref="B97:B110"/>
     </sheetView>
   </sheetViews>

</xml_diff>